<commit_message>
TMT0072201_TMT0072203_TMT0072205_TMT0072207_TMT0072209_VerifyThatDelegateOfPrimaryAttendeeCan_Add_View_Edit_SendNotification_Delete_TheActivity - Initial - 3 Oct 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032670_VerifyThatDelegateOfPrimaryAttendeeCan_Add_View_Edit_SendNotification_Delete_TheActivity.xlsx
+++ b/TestData/TMTC0032670_VerifyThatDelegateOfPrimaryAttendeeCan_Add_View_Edit_SendNotification_Delete_TheActivity.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C68EF3-158E-43EA-9AFA-A90063FAF87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02798437-D1C5-4C15-8D2B-076E3E226336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
-    <sheet name="Contact" sheetId="10" r:id="rId2"/>
-    <sheet name="Activity" sheetId="11" r:id="rId3"/>
-    <sheet name="MoreAttendees" sheetId="12" r:id="rId4"/>
+    <sheet name="UpdateActivity" sheetId="13" r:id="rId2"/>
+    <sheet name="Contact" sheetId="10" r:id="rId3"/>
+    <sheet name="Activity" sheetId="11" r:id="rId4"/>
+    <sheet name="MoreAttendees" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Type</t>
   </si>
@@ -114,6 +115,24 @@
   </si>
   <si>
     <t>Delegate Meeting Description 1</t>
+  </si>
+  <si>
+    <t>FIG - Financial Institutions</t>
+  </si>
+  <si>
+    <t>Advisory</t>
+  </si>
+  <si>
+    <t>Updated Notes</t>
+  </si>
+  <si>
+    <t>Amanda Donovan</t>
+  </si>
+  <si>
+    <t>Updated By Delegate</t>
+  </si>
+  <si>
+    <t>Updated By Delegate Description</t>
   </si>
 </sst>
 </file>
@@ -451,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,6 +496,76 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD5835D-A731-4749-8B8C-898BB7148BBB}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F6AD56-19A8-4526-A92B-5BB161C99B6D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -518,7 +607,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB9990D-2177-413E-8716-FEF5A04433C7}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -590,7 +679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FD42B5-FCC0-46AF-9C9E-BDDDE197E6BE}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Activities Delegate - 3 Oct 2024 - Final
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032670_VerifyThatDelegateOfPrimaryAttendeeCan_Add_View_Edit_SendNotification_Delete_TheActivity.xlsx
+++ b/TestData/TMTC0032670_VerifyThatDelegateOfPrimaryAttendeeCan_Add_View_Edit_SendNotification_Delete_TheActivity.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02798437-D1C5-4C15-8D2B-076E3E226336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D0E700-DA82-4F6D-B431-7CD1B0CFD33F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
-    <sheet name="UpdateActivity" sheetId="13" r:id="rId2"/>
-    <sheet name="Contact" sheetId="10" r:id="rId3"/>
-    <sheet name="Activity" sheetId="11" r:id="rId4"/>
-    <sheet name="MoreAttendees" sheetId="12" r:id="rId5"/>
+    <sheet name="Contact" sheetId="10" r:id="rId2"/>
+    <sheet name="Activity" sheetId="11" r:id="rId3"/>
+    <sheet name="MoreAttendees" sheetId="12" r:id="rId4"/>
+    <sheet name="Notification" sheetId="14" r:id="rId5"/>
+    <sheet name="UpdateActivity" sheetId="13" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Type</t>
   </si>
@@ -133,6 +134,9 @@
   </si>
   <si>
     <t>Updated By Delegate Description</t>
+  </si>
+  <si>
+    <t>Email ID</t>
   </si>
 </sst>
 </file>
@@ -496,11 +500,185 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F6AD56-19A8-4526-A92B-5BB161C99B6D}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB9990D-2177-413E-8716-FEF5A04433C7}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FD42B5-FCC0-46AF-9C9E-BDDDE197E6BE}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F30D569-3C20-422F-B8AB-7FCD9ED58AD6}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD5835D-A731-4749-8B8C-898BB7148BBB}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,153 +741,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F6AD56-19A8-4526-A92B-5BB161C99B6D}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB9990D-2177-413E-8716-FEF5A04433C7}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FD42B5-FCC0-46AF-9C9E-BDDDE197E6BE}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>